<commit_message>
finished the magical 21 question
</commit_message>
<xml_diff>
--- a/questions_points.xlsx
+++ b/questions_points.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kruppajo/work/GitHub/exam/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1F2066A1-0D48-A34B-BB86-FFC7783A6E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{66934E68-C849-8744-96B1-D1C3F9B9EE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5980" yWindow="500" windowWidth="18280" windowHeight="15360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1165,8 +1165,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD30"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1859,7 +1859,7 @@
         <v>88</v>
       </c>
       <c r="B86">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
new exams and bugs
</commit_message>
<xml_diff>
--- a/questions_points.xlsx
+++ b/questions_points.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jokruppa\Documents\GitHub\exam\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kruppajo/work/GitHub/exam/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3360B14C-55CB-442D-8B7C-094696B19B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3D8C6E1C-69ED-144D-900E-EBE483D42EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="30960" windowHeight="12312" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="30960" windowHeight="15780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="questions_points" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="82" uniqueCount="82">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="83" uniqueCount="83">
   <si>
     <t>file_name</t>
   </si>
@@ -282,6 +282,9 @@
   </si>
   <si>
     <t>desc_stat-13.Rnw</t>
+  </si>
+  <si>
+    <t>ttest-08.Rnw</t>
   </si>
 </sst>
 </file>
@@ -845,9 +848,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -885,7 +888,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -991,7 +994,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1133,7 +1136,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1141,18 +1144,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B81"/>
+  <dimension ref="A1:B82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1160,7 +1163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -1168,7 +1171,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -1176,7 +1179,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>72</v>
       </c>
@@ -1184,7 +1187,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -1192,7 +1195,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -1200,7 +1203,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>75</v>
       </c>
@@ -1208,7 +1211,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>76</v>
       </c>
@@ -1216,7 +1219,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -1224,7 +1227,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>78</v>
       </c>
@@ -1232,7 +1235,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>79</v>
       </c>
@@ -1240,7 +1243,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>80</v>
       </c>
@@ -1248,7 +1251,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -1256,7 +1259,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1264,7 +1267,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1272,7 +1275,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1280,7 +1283,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1288,7 +1291,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1296,7 +1299,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1304,504 +1307,512 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>32</v>
       </c>
       <c r="B20">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>33</v>
       </c>
       <c r="B21">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>34</v>
       </c>
       <c r="B22">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>35</v>
       </c>
       <c r="B23">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>36</v>
       </c>
       <c r="B24">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>37</v>
       </c>
       <c r="B25">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="B26">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>39</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>40</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>41</v>
       </c>
-      <c r="B29">
+      <c r="B30">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>42</v>
       </c>
-      <c r="B30">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="B31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>43</v>
-      </c>
-      <c r="B31">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>44</v>
       </c>
       <c r="B32">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>45</v>
       </c>
-      <c r="B33">
+      <c r="B34">
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>46</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>47</v>
       </c>
-      <c r="B35">
+      <c r="B36">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>48</v>
       </c>
-      <c r="B36">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="B37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>49</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>50</v>
       </c>
-      <c r="B38">
+      <c r="B39">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>51</v>
       </c>
-      <c r="B39">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="B40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>52</v>
       </c>
-      <c r="B40">
+      <c r="B41">
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>59</v>
       </c>
-      <c r="B41">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="B42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>60</v>
       </c>
-      <c r="B42">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="B43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>61</v>
       </c>
-      <c r="B43">
+      <c r="B44">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>62</v>
-      </c>
-      <c r="B44">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>63</v>
       </c>
       <c r="B45">
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>64</v>
       </c>
-      <c r="B46">
+      <c r="B47">
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>65</v>
       </c>
-      <c r="B47">
+      <c r="B48">
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>66</v>
       </c>
-      <c r="B48">
+      <c r="B49">
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>67</v>
       </c>
-      <c r="B49">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="B50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>68</v>
       </c>
-      <c r="B50">
+      <c r="B51">
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>69</v>
       </c>
-      <c r="B51">
+      <c r="B52">
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>53</v>
       </c>
-      <c r="B52">
+      <c r="B53">
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>58</v>
       </c>
-      <c r="B53">
+      <c r="B54">
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>57</v>
       </c>
-      <c r="B54">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="B55">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>54</v>
-      </c>
-      <c r="B55">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>56</v>
       </c>
       <c r="B56">
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>55</v>
       </c>
-      <c r="B57">
+      <c r="B58">
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>2</v>
       </c>
-      <c r="B58">
+      <c r="B59">
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>23</v>
       </c>
-      <c r="B59">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+      <c r="B60">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>3</v>
       </c>
-      <c r="B60">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="B61">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>4</v>
       </c>
-      <c r="B61">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+      <c r="B62">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>5</v>
       </c>
-      <c r="B62">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+      <c r="B63">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>6</v>
       </c>
-      <c r="B63">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+      <c r="B64">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>7</v>
       </c>
-      <c r="B64">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+      <c r="B65">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>8</v>
       </c>
-      <c r="B65">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+      <c r="B66">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>9</v>
       </c>
-      <c r="B66">
+      <c r="B67">
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>10</v>
-      </c>
-      <c r="B67">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>11</v>
       </c>
-      <c r="B68">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+      <c r="B69">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>12</v>
       </c>
-      <c r="B69">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+      <c r="B70">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>13</v>
       </c>
-      <c r="B70">
+      <c r="B71">
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>14</v>
       </c>
-      <c r="B71">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+      <c r="B72">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>15</v>
       </c>
-      <c r="B72">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+      <c r="B73">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>16</v>
       </c>
-      <c r="B73">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
+      <c r="B74">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>17</v>
       </c>
-      <c r="B74">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+      <c r="B75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>21</v>
-      </c>
-      <c r="B75">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>22</v>
       </c>
       <c r="B76">
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>22</v>
+      </c>
+      <c r="B77">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>24</v>
       </c>
-      <c r="B77">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
+      <c r="B78">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>25</v>
       </c>
-      <c r="B78">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+      <c r="B79">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>18</v>
       </c>
-      <c r="B79">
+      <c r="B80">
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>19</v>
       </c>
-      <c r="B80">
+      <c r="B81">
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>20</v>
       </c>
-      <c r="B81">
+      <c r="B82">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B81">
+  <conditionalFormatting sqref="B2:B82">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>7</formula>
     </cfRule>

</xml_diff>

<commit_message>
cleaning of non-used exams
</commit_message>
<xml_diff>
--- a/questions_points.xlsx
+++ b/questions_points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kruppajo/work/GitHub/exam/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1E6D5681-6B37-3D42-A58F-924E26719755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5007EC27-0502-294A-A5C1-218BC1F94A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="760" windowWidth="30960" windowHeight="15780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="84" uniqueCount="84">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="80" uniqueCount="80">
   <si>
     <t>file_name</t>
   </si>
@@ -191,9 +191,6 @@
     <t>chisquare-05.Rnw</t>
   </si>
   <si>
-    <t>chisquare-06.Rnw</t>
-  </si>
-  <si>
     <t>linreg-01.Rnw</t>
   </si>
   <si>
@@ -237,15 +234,6 @@
   </si>
   <si>
     <t>linreg-09.Rnw</t>
-  </si>
-  <si>
-    <t>linreg-10.Rnw</t>
-  </si>
-  <si>
-    <t>linreg-11.Rnw</t>
-  </si>
-  <si>
-    <t>linreg-12.Rnw</t>
   </si>
   <si>
     <t>desc_stat-01.Rnw</t>
@@ -1147,10 +1135,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B83"/>
+  <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1168,7 +1156,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -1176,7 +1164,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B3">
         <v>7</v>
@@ -1184,7 +1172,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -1192,7 +1180,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B5">
         <v>9</v>
@@ -1200,7 +1188,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -1208,7 +1196,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B7">
         <v>8</v>
@@ -1216,7 +1204,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B8">
         <v>8</v>
@@ -1224,7 +1212,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B9">
         <v>10</v>
@@ -1232,7 +1220,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B10">
         <v>8</v>
@@ -1240,7 +1228,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -1248,7 +1236,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B12">
         <v>9</v>
@@ -1256,7 +1244,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B13">
         <v>9</v>
@@ -1360,7 +1348,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B26">
         <v>8</v>
@@ -1432,7 +1420,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B35">
         <v>9</v>
@@ -1483,15 +1471,15 @@
         <v>51</v>
       </c>
       <c r="B41">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B42">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -1507,7 +1495,7 @@
         <v>60</v>
       </c>
       <c r="B44">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -1515,7 +1503,7 @@
         <v>61</v>
       </c>
       <c r="B45">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -1523,7 +1511,7 @@
         <v>62</v>
       </c>
       <c r="B46">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -1531,7 +1519,7 @@
         <v>63</v>
       </c>
       <c r="B47">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -1547,100 +1535,100 @@
         <v>65</v>
       </c>
       <c r="B49">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B50">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B51">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B52">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B53">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B54">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B55">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>2</v>
       </c>
       <c r="B56">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="B57">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="B58">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="B59">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B60">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B61">
         <v>10</v>
@@ -1648,7 +1636,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B62">
         <v>10</v>
@@ -1656,7 +1644,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B63">
         <v>10</v>
@@ -1664,15 +1652,15 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B64">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B65">
         <v>10</v>
@@ -1680,7 +1668,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B66">
         <v>10</v>
@@ -1688,7 +1676,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B67">
         <v>10</v>
@@ -1696,7 +1684,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B68">
         <v>12</v>
@@ -1704,7 +1692,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B69">
         <v>10</v>
@@ -1712,7 +1700,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B70">
         <v>10</v>
@@ -1720,7 +1708,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B71">
         <v>10</v>
@@ -1728,31 +1716,31 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B72">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B73">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B74">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B75">
         <v>10</v>
@@ -1760,7 +1748,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B76">
         <v>10</v>
@@ -1768,62 +1756,30 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B77">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B78">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B79">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>25</v>
-      </c>
-      <c r="B80">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>18</v>
-      </c>
-      <c r="B81">
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>19</v>
-      </c>
-      <c r="B82">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>20</v>
-      </c>
-      <c r="B83">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B83">
+  <conditionalFormatting sqref="B2:B79">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>7</formula>
     </cfRule>

</xml_diff>

<commit_message>
better exams with RNG
</commit_message>
<xml_diff>
--- a/questions_points.xlsx
+++ b/questions_points.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kruppajo/work/GitHub/exam/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E7BE5699-080D-1E48-830D-37BECFF62CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{EEFDB2C7-F1C3-1B45-B6CD-21BCC538C920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40620" yWindow="3920" windowWidth="18640" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8040" yWindow="4240" windowWidth="18640" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="questions_points" sheetId="1" r:id="rId1"/>
@@ -1140,8 +1140,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="245" zoomScaleNormal="245" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1210,7 +1210,7 @@
         <v>70</v>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added and reworked MC questions
</commit_message>
<xml_diff>
--- a/questions_points.xlsx
+++ b/questions_points.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kruppajo/work/GitHub/exam/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{EE555566-78CC-C648-AC12-EDC59FF53705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{52D5A984-4657-5F47-B5A1-03DEF78DAA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12220" yWindow="5420" windowWidth="24160" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="84" uniqueCount="84">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="82" uniqueCount="82">
   <si>
     <t>file_name</t>
   </si>
@@ -240,12 +240,6 @@
   </si>
   <si>
     <t>desc_stat-08.Rnw</t>
-  </si>
-  <si>
-    <t>desc_stat-10.Rnw</t>
-  </si>
-  <si>
-    <t>desc_stat-11.Rnw</t>
   </si>
   <si>
     <t>ttest-08.Rnw</t>
@@ -1157,10 +1151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B83"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1242,7 +1236,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B10">
         <v>10</v>
@@ -1250,39 +1244,39 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="B13">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="B14">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B15">
         <v>9</v>
@@ -1290,39 +1284,39 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B16">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B17">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B18">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B19">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B20">
         <v>12</v>
@@ -1330,39 +1324,39 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B21">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B22">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B23">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B24">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="B25">
         <v>10</v>
@@ -1370,31 +1364,31 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B26">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="B27">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B28">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B29">
         <v>9</v>
@@ -1402,7 +1396,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B30">
         <v>12</v>
@@ -1410,15 +1404,15 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B31">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B32">
         <v>12</v>
@@ -1426,39 +1420,39 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B33">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="B34">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B35">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="B36">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B37">
         <v>10</v>
@@ -1466,7 +1460,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B38">
         <v>10</v>
@@ -1474,7 +1468,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B39">
         <v>10</v>
@@ -1482,79 +1476,79 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="B40">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="B41">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="B42">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="B43">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B44">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B45">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B46">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B47">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B48">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B49">
         <v>12</v>
@@ -1562,42 +1556,42 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B50">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B51">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B52">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="B53">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="B54">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -1605,7 +1599,7 @@
         <v>75</v>
       </c>
       <c r="B55">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -1613,7 +1607,7 @@
         <v>76</v>
       </c>
       <c r="B56">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -1621,28 +1615,28 @@
         <v>77</v>
       </c>
       <c r="B57">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>78</v>
+        <v>2</v>
       </c>
       <c r="B58">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>79</v>
+        <v>23</v>
       </c>
       <c r="B59">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B60">
         <v>10</v>
@@ -1650,7 +1644,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B61">
         <v>10</v>
@@ -1658,7 +1652,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B62">
         <v>10</v>
@@ -1666,7 +1660,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B63">
         <v>10</v>
@@ -1674,7 +1668,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B64">
         <v>10</v>
@@ -1682,7 +1676,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B65">
         <v>10</v>
@@ -1690,7 +1684,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B66">
         <v>10</v>
@@ -1698,7 +1692,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B67">
         <v>10</v>
@@ -1706,7 +1700,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B68">
         <v>10</v>
@@ -1714,7 +1708,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B69">
         <v>10</v>
@@ -1722,7 +1716,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B70">
         <v>10</v>
@@ -1730,7 +1724,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B71">
         <v>10</v>
@@ -1738,15 +1732,15 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B72">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B73">
         <v>10</v>
@@ -1754,39 +1748,39 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B74">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B75">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B76">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="B77">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="B78">
         <v>12</v>
@@ -1794,46 +1788,30 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="B79">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>74</v>
+        <v>19</v>
       </c>
       <c r="B80">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B81">
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>19</v>
-      </c>
-      <c r="B82">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>20</v>
-      </c>
-      <c r="B83">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B83">
+  <conditionalFormatting sqref="B2:B81">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>9</formula>
     </cfRule>

</xml_diff>